<commit_message>
Uodated the sequence of instruments in research_facilities.xlsx
</commit_message>
<xml_diff>
--- a/research_facilities.xlsx
+++ b/research_facilities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\CSPIT_Main\CSPIT_NEW_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motat\OneDrive\Desktop\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E272AF-389D-43CA-ADDD-048D87B1C5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A55793-549A-4CF8-B6A7-F5D3281D622E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -348,12 +348,6 @@
     <t>Mechanical</t>
   </si>
   <si>
-    <t>images1\facilities\Mech\mech1.png</t>
-  </si>
-  <si>
-    <t>images1\facilities\Mech\mech2.png</t>
-  </si>
-  <si>
     <t>Advanced Programming Lab: </t>
   </si>
   <si>
@@ -729,6 +723,12 @@
   </si>
   <si>
     <t>images1\facilities\EE\Power Quality Analyzer.webp</t>
+  </si>
+  <si>
+    <t>images1\facilities\Mech\mech1.webp</t>
+  </si>
+  <si>
+    <t>images1\facilities\Mech\mech2.webp</t>
   </si>
 </sst>
 </file>
@@ -842,7 +842,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -886,6 +886,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1170,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32:E65"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1201,1167 +1204,1169 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>95</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>95</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="22.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>95</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="91.8" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>95</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>18</v>
+        <v>95</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>25</v>
+        <v>111</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>26</v>
+        <v>95</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>49</v>
+        <v>112</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>95</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>50</v>
+        <v>112</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>95</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>95</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="112.2" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>95</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>95</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>95</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>55</v>
+        <v>112</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>95</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>56</v>
+        <v>112</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>95</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>57</v>
+        <v>112</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="B26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="112.2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="173.4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="163.19999999999999" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>114</v>
-      </c>
       <c r="E30" s="10" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>73</v>
+        <v>113</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30.6" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>74</v>
+      <c r="B32" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30.6" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>75</v>
+      <c r="B33" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>149</v>
+        <v>112</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>76</v>
+        <v>113</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>77</v>
+      <c r="B35" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>78</v>
+      <c r="B36" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D36" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>79</v>
+      <c r="B37" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="173.4" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D37" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>80</v>
+      <c r="B38" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>81</v>
+      <c r="B39" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D39" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>82</v>
+      <c r="B40" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="163.19999999999999" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D40" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E40" s="15" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>83</v>
+      <c r="B41" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>157</v>
+        <v>128</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>84</v>
+        <v>113</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E42" s="15" t="s">
-        <v>158</v>
+        <v>112</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>85</v>
+        <v>113</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>159</v>
+        <v>112</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>86</v>
+        <v>113</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D44" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>87</v>
+      <c r="B45" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D45" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>26</v>
+      <c r="B46" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>88</v>
+      <c r="B47" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D47" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>89</v>
+      <c r="B48" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>90</v>
+        <v>112</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="244.8" x14ac:dyDescent="0.2">
+      <c r="A49" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>102</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>114</v>
+        <v>138</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>139</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>91</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="173.4" x14ac:dyDescent="0.2">
+      <c r="A50" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>103</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>117</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>92</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>110</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>114</v>
+        <v>118</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>119</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>93</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="153" x14ac:dyDescent="0.2">
+      <c r="A52" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>104</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>121</v>
       </c>
       <c r="E52" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E53" s="15" t="s">
+    <row r="54" spans="1:5" ht="173.4" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E54" s="15" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B54" s="11" t="s">
+    <row r="55" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D54" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="E54" s="15" t="s">
+      <c r="D55" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E55" s="15" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="173.4" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B55" s="11" t="s">
+    <row r="56" spans="1:5" ht="112.2" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D55" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="E55" s="15" t="s">
+      <c r="D56" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="E56" s="15" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B56" s="11" t="s">
+    <row r="57" spans="1:5" ht="255" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D56" s="14" t="s">
+      <c r="C57" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D57" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E56" s="15" t="s">
+      <c r="E57" s="15" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="112.2" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="E57" s="15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="255" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>102</v>
+    <row r="58" spans="1:5" ht="61.2" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D58" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="244.8" x14ac:dyDescent="0.2">
-      <c r="A59" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B59" s="13" t="s">
-        <v>104</v>
+        <v>8</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="91.8" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D59" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="E59" s="15" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="173.4" x14ac:dyDescent="0.2">
-      <c r="A60" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>105</v>
+        <v>10</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="132.6" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="81.599999999999994" x14ac:dyDescent="0.2">
-      <c r="A61" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>112</v>
+        <v>13</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="91.8" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="E61" s="15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="153" x14ac:dyDescent="0.2">
-      <c r="A62" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B62" s="13" t="s">
-        <v>106</v>
+        <v>16</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>180</v>
+        <v>19</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="112.2" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="112.2" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="112.2" x14ac:dyDescent="0.2">
       <c r="A65" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{572BA000-D83C-4FD3-B3AF-7AFAC9687069}"/>
-    <hyperlink ref="E3:E6" r:id="rId2" display="images1\facilities\IT\IT_1.webp" xr:uid="{DEF6C1D5-55C0-4567-87AB-2160B05F4505}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{509855C7-E1F4-4516-BBD3-D5C8C114DA2A}"/>
-    <hyperlink ref="E4" r:id="rId4" xr:uid="{C8CD4369-6D56-4659-B5FE-7BA2E74C9C56}"/>
-    <hyperlink ref="E5" r:id="rId5" xr:uid="{54F4D55E-B8EE-4221-B006-C4B4DFE9C83C}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{C270C5B0-C9BF-4454-9650-0207DA920BA7}"/>
-    <hyperlink ref="E7" r:id="rId7" xr:uid="{EDD4D942-9A1C-4F69-BF56-B9DE75586232}"/>
-    <hyperlink ref="E8:E29" r:id="rId8" display="images1\facilities\CL\cl1.webp" xr:uid="{C11EA648-1296-46E3-B49F-6C175435FC7F}"/>
-    <hyperlink ref="E8" r:id="rId9" xr:uid="{4384D672-7CBE-4651-A630-998D8BC4CB37}"/>
-    <hyperlink ref="E9" r:id="rId10" xr:uid="{574BAD2A-96B1-49B3-99A4-9594F5207A5C}"/>
-    <hyperlink ref="E10" r:id="rId11" xr:uid="{DE3CBA4E-603B-4914-A655-496EAA893020}"/>
-    <hyperlink ref="E11" r:id="rId12" xr:uid="{E581F71E-1D48-4FE7-82E4-C25E13DD9D73}"/>
-    <hyperlink ref="E12" r:id="rId13" xr:uid="{D9E2C6B8-9CCC-452D-9C05-AFDAC6EA3321}"/>
-    <hyperlink ref="E13" r:id="rId14" xr:uid="{5B7493DC-2811-4483-BBF7-46E801B02442}"/>
-    <hyperlink ref="E14" r:id="rId15" xr:uid="{86AC93C9-BA3F-4D08-9DF9-D7091439FC89}"/>
-    <hyperlink ref="E15" r:id="rId16" xr:uid="{525E8591-B04C-4EB9-858A-16524D753247}"/>
-    <hyperlink ref="E16" r:id="rId17" xr:uid="{57A24FC3-62F2-402B-A407-771B4BCD8023}"/>
-    <hyperlink ref="E17" r:id="rId18" xr:uid="{D7D569EF-4DFE-4226-9055-C3F6B2D9A934}"/>
-    <hyperlink ref="E18" r:id="rId19" xr:uid="{DC16B157-5114-4AA8-A267-AADAFD7624BF}"/>
-    <hyperlink ref="E19" r:id="rId20" xr:uid="{41217E53-AEC8-456E-A2A6-E091CA864992}"/>
-    <hyperlink ref="E20" r:id="rId21" xr:uid="{160BBDE3-22F9-4F55-8D97-B57ABEE3C5A3}"/>
-    <hyperlink ref="E21" r:id="rId22" xr:uid="{9969F231-53E6-4439-A30F-CB28912107F5}"/>
-    <hyperlink ref="E22" r:id="rId23" xr:uid="{0A23C2A6-8EAF-46BD-9565-1B690795E8F0}"/>
-    <hyperlink ref="E23" r:id="rId24" xr:uid="{3CEB9446-0ED4-4660-9675-F4360AF62639}"/>
-    <hyperlink ref="E24" r:id="rId25" xr:uid="{A9087166-08E4-40A1-9A4B-4C63E67DA3F3}"/>
-    <hyperlink ref="E25" r:id="rId26" xr:uid="{3C05F0A2-BBCD-4244-8F51-F8F7DC0E12C0}"/>
-    <hyperlink ref="E26" r:id="rId27" xr:uid="{776C1C53-E31E-44A2-8F39-CC1EE622633C}"/>
-    <hyperlink ref="E27" r:id="rId28" xr:uid="{D1FF9C55-1587-4FC0-AF90-A4BDBAC8DA1B}"/>
-    <hyperlink ref="E28" r:id="rId29" xr:uid="{7BBD9408-CA3D-4AC4-81D5-8E4374B8C1AA}"/>
-    <hyperlink ref="E29" r:id="rId30" xr:uid="{A03BCCD0-524B-496B-AD59-000634981CB8}"/>
-    <hyperlink ref="E30" r:id="rId31" xr:uid="{3EBA9268-9557-4A48-8B84-CAC90FC413E5}"/>
-    <hyperlink ref="E31" r:id="rId32" xr:uid="{9F8FBCCA-CF97-4390-AF4A-61C45873D9CB}"/>
-    <hyperlink ref="E63:E65" r:id="rId33" display="https://placehold.co/600x400" xr:uid="{9DECB28C-E304-42CD-B2E9-4B22F3DAE36B}"/>
-    <hyperlink ref="E32:E62" r:id="rId34" display="https://placehold.co/600x400" xr:uid="{CB3108AF-EBD3-416A-89E3-20D7365301DC}"/>
-    <hyperlink ref="E32" r:id="rId35" xr:uid="{2F02F380-5A2F-4E54-A2B0-B00B0B5474BF}"/>
-    <hyperlink ref="E33" r:id="rId36" xr:uid="{3F0EFEA8-698B-4D75-B445-6BFC86F886EF}"/>
-    <hyperlink ref="E34" r:id="rId37" xr:uid="{5304E0D3-1292-4331-96E9-D22A65B78694}"/>
-    <hyperlink ref="E35" r:id="rId38" xr:uid="{B5FACA71-F097-4AEA-98AB-D5CB68183368}"/>
-    <hyperlink ref="E36" r:id="rId39" xr:uid="{3A0BE742-14BF-49E4-8E70-330451AB8E81}"/>
-    <hyperlink ref="E37" r:id="rId40" xr:uid="{9603DA2B-4450-4C1D-913F-E5496AB877F9}"/>
-    <hyperlink ref="E38" r:id="rId41" xr:uid="{A9D98258-59EB-4D43-8CA5-CB11A5C5A774}"/>
-    <hyperlink ref="E39" r:id="rId42" xr:uid="{EE6678ED-163E-403E-8E1D-32C81A252308}"/>
-    <hyperlink ref="E40" r:id="rId43" xr:uid="{3C3C9BE2-160E-4D68-A207-5E379E50D522}"/>
-    <hyperlink ref="E41" r:id="rId44" xr:uid="{05E38872-6560-46C6-B712-28F6FF507EDD}"/>
-    <hyperlink ref="E42" r:id="rId45" xr:uid="{419DC80D-6B60-40F8-A9E1-8E222B669DA2}"/>
-    <hyperlink ref="E43" r:id="rId46" xr:uid="{E37EDAD8-FF96-41C6-BC2F-E987CDD7A4F6}"/>
-    <hyperlink ref="E44" r:id="rId47" xr:uid="{64D3B60F-1D38-4BBD-A4E0-404B1A8C9540}"/>
-    <hyperlink ref="E45" r:id="rId48" xr:uid="{9F69CB29-E788-4BEC-8F8A-3551D3BD2341}"/>
-    <hyperlink ref="E47" r:id="rId49" xr:uid="{80AE7065-EBCD-480B-9829-489A2985AA51}"/>
-    <hyperlink ref="E46" r:id="rId50" xr:uid="{4A3B3757-A3DD-4D9B-A9BB-3FA690198B63}"/>
-    <hyperlink ref="E48" r:id="rId51" xr:uid="{55E2A029-D53E-4D43-8173-6165E31D35AE}"/>
-    <hyperlink ref="E49" r:id="rId52" xr:uid="{B063A0B1-7E52-4935-A1B2-548C5DA274B3}"/>
-    <hyperlink ref="E50" r:id="rId53" xr:uid="{5783713B-9D7C-4700-BAD5-C3661D5723C4}"/>
-    <hyperlink ref="E51" r:id="rId54" xr:uid="{C4609A61-E05A-4424-A18F-08BB4D89D08D}"/>
-    <hyperlink ref="E52" r:id="rId55" xr:uid="{21550780-4893-4667-BD21-AA0151056F43}"/>
-    <hyperlink ref="E53" r:id="rId56" xr:uid="{2BBCBBDA-7AEF-48CC-B58E-ED6ACF07C58F}"/>
-    <hyperlink ref="E54" r:id="rId57" xr:uid="{AE256692-E686-4080-A7AB-0FEB205F6D29}"/>
-    <hyperlink ref="E55" r:id="rId58" xr:uid="{84E3E7DC-884C-49FD-9B25-0FBE8FBCF48A}"/>
-    <hyperlink ref="E56" r:id="rId59" xr:uid="{0FCE16BC-D540-4257-936B-1D7E3CE4650C}"/>
-    <hyperlink ref="E57" r:id="rId60" xr:uid="{2A5DDE93-F7F2-4B57-920F-5CF16260C0C0}"/>
-    <hyperlink ref="E58" r:id="rId61" xr:uid="{66F0CDCD-1420-43CF-A9E2-BC1AC545A21E}"/>
-    <hyperlink ref="E63" r:id="rId62" xr:uid="{68158914-939C-4F54-901A-C4E7A6CD26E6}"/>
-    <hyperlink ref="E64" r:id="rId63" xr:uid="{070000AE-5AFA-4374-B510-B5DDB65C1B85}"/>
-    <hyperlink ref="E65" r:id="rId64" xr:uid="{C1354424-A16E-4127-A382-E761D1EC05A3}"/>
-    <hyperlink ref="E59" r:id="rId65" xr:uid="{6339267F-6784-4D32-AF1B-6B9161AD2DCA}"/>
-    <hyperlink ref="E60" r:id="rId66" xr:uid="{001F1D9D-87EB-407E-8952-BD41ED689541}"/>
-    <hyperlink ref="E61" r:id="rId67" xr:uid="{A40B1394-2C0D-4C60-8C58-6DBEA24CB7D6}"/>
-    <hyperlink ref="E62" r:id="rId68" xr:uid="{302C620F-0551-4BEC-AE6A-EFEFB4A5A02F}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{B6EAEAEC-2327-4740-B423-9592DB73C7CA}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{573D4282-9065-4DCD-8963-3F1F5F44591C}"/>
+    <hyperlink ref="E4:E25" r:id="rId3" display="https://placehold.co/600x400" xr:uid="{19A02284-3928-4D5D-9C76-E96E324616AA}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{88933416-69CD-400F-8DB1-22060C1A759E}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{D443AFDB-0702-4E6A-B01B-72A7701D6AF7}"/>
+    <hyperlink ref="E6" r:id="rId6" xr:uid="{5B141F52-4130-4D06-99B5-59CB5EF05D8B}"/>
+    <hyperlink ref="E7" r:id="rId7" xr:uid="{BFBDFDF9-FE5C-46DB-8DC1-08E999C5E3B9}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{8C75CE57-8442-4A9E-9B61-07A134AEF6CE}"/>
+    <hyperlink ref="E9" r:id="rId9" xr:uid="{DD48FDC9-C855-4276-8138-C317B406B850}"/>
+    <hyperlink ref="E10" r:id="rId10" xr:uid="{5EF9136B-7B59-462B-9ED6-04620B5D2225}"/>
+    <hyperlink ref="E11" r:id="rId11" xr:uid="{C5997A75-9E02-4889-93F6-D9DD6440394B}"/>
+    <hyperlink ref="E12" r:id="rId12" xr:uid="{CE7B2DFF-CEC4-43B3-89EC-4BB88446A5D5}"/>
+    <hyperlink ref="E13" r:id="rId13" xr:uid="{65AC3B30-8170-493C-ADAC-F3BBF836ECAE}"/>
+    <hyperlink ref="E14" r:id="rId14" xr:uid="{CDFEA37C-CE9F-411D-A8C5-47E982C73303}"/>
+    <hyperlink ref="E15" r:id="rId15" xr:uid="{4823E0C1-00A1-4D25-AF28-F9CB3F423C9E}"/>
+    <hyperlink ref="E16" r:id="rId16" xr:uid="{8105D3D4-BA2E-466F-A031-578EE633BCE8}"/>
+    <hyperlink ref="E17" r:id="rId17" xr:uid="{5FD07EBD-CC4B-4AAA-89AD-DA38ADFA8080}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{BE9CC2A7-4086-4B42-AF25-5DEDF2972499}"/>
+    <hyperlink ref="E18" r:id="rId19" xr:uid="{31EE4361-A415-4F6A-A866-A5BC9DC6432A}"/>
+    <hyperlink ref="E20" r:id="rId20" xr:uid="{B078794E-A907-4A0F-89A0-1F40BB7D0791}"/>
+    <hyperlink ref="E21" r:id="rId21" xr:uid="{CAD48FB3-5288-48B1-8526-31A45F820262}"/>
+    <hyperlink ref="E22" r:id="rId22" xr:uid="{5932967D-5888-4141-9AFC-231F56DBA886}"/>
+    <hyperlink ref="E23" r:id="rId23" xr:uid="{8155F7DF-4E25-414F-949B-AACEA6D0FA12}"/>
+    <hyperlink ref="E24" r:id="rId24" xr:uid="{4087A646-2F7A-4397-9603-861E4B929676}"/>
+    <hyperlink ref="E25" r:id="rId25" xr:uid="{D739F527-3285-4FFF-BFF2-D0CC704FFAC5}"/>
+    <hyperlink ref="E26" r:id="rId26" xr:uid="{6C7E9892-37EA-4E00-B7A1-B6A0F6C221B9}"/>
+    <hyperlink ref="E27:E48" r:id="rId27" display="images1\facilities\CL\cl1.webp" xr:uid="{0E4D0FEC-D74B-45A0-9367-BD8C5F7A5D60}"/>
+    <hyperlink ref="E27" r:id="rId28" xr:uid="{E7D2E82D-1D3E-4FEF-8991-806138E50485}"/>
+    <hyperlink ref="E28" r:id="rId29" xr:uid="{608F641D-E667-46BC-8449-64FFDAC4E7FE}"/>
+    <hyperlink ref="E29" r:id="rId30" xr:uid="{D3158DB9-7341-400C-B7EA-0397ABD5F9C2}"/>
+    <hyperlink ref="E30" r:id="rId31" xr:uid="{CF78BF8B-674C-43D5-9920-7CD87F8EAACC}"/>
+    <hyperlink ref="E31" r:id="rId32" xr:uid="{94928AC6-9E3A-46E3-A550-7B2A90EEE1D3}"/>
+    <hyperlink ref="E32" r:id="rId33" xr:uid="{DE7B2FBB-D16F-4FE9-A2D2-C2324777CB28}"/>
+    <hyperlink ref="E33" r:id="rId34" xr:uid="{75CA24C4-E4E4-43EF-82B6-F21AA7E4566B}"/>
+    <hyperlink ref="E34" r:id="rId35" xr:uid="{FFE48F25-D362-4A50-9320-88D5C6287ACB}"/>
+    <hyperlink ref="E35" r:id="rId36" xr:uid="{6FABB0F0-62FF-41D2-B9FA-47DAD8D97042}"/>
+    <hyperlink ref="E36" r:id="rId37" xr:uid="{B406963A-F5DB-4BEB-ADF6-486D6EB8ACF0}"/>
+    <hyperlink ref="E37" r:id="rId38" xr:uid="{5503DB04-F071-4921-8043-264EB8021A6D}"/>
+    <hyperlink ref="E38" r:id="rId39" xr:uid="{4922ACD1-FEE8-4E69-8DBF-10693195CC56}"/>
+    <hyperlink ref="E39" r:id="rId40" xr:uid="{9289519F-A579-443A-B712-147A47D85D07}"/>
+    <hyperlink ref="E40" r:id="rId41" xr:uid="{982E21B8-0135-43D5-93C7-6D1986897AFD}"/>
+    <hyperlink ref="E41" r:id="rId42" xr:uid="{3C147460-1153-4848-8C7C-E50147491C6B}"/>
+    <hyperlink ref="E42" r:id="rId43" xr:uid="{971CAA82-6B70-495A-A875-4423FACF0EAC}"/>
+    <hyperlink ref="E43" r:id="rId44" xr:uid="{45BD2842-6B08-4F96-A3D2-B453713FD4C5}"/>
+    <hyperlink ref="E44" r:id="rId45" xr:uid="{FF906FCB-862F-4D1D-AC96-C3161F3575B1}"/>
+    <hyperlink ref="E45" r:id="rId46" xr:uid="{66D927EC-096C-4E10-A142-4A4AE0E4C3C3}"/>
+    <hyperlink ref="E46" r:id="rId47" xr:uid="{99008226-90DF-4CCE-A5B4-3A4E2C7AA647}"/>
+    <hyperlink ref="E47" r:id="rId48" xr:uid="{539B662E-A8E4-4E41-806B-964987557371}"/>
+    <hyperlink ref="E48" r:id="rId49" xr:uid="{6CF1056B-233A-440D-B58B-A6012B35F06B}"/>
+    <hyperlink ref="E49:E52" r:id="rId50" display="https://placehold.co/600x400" xr:uid="{E55F2068-9588-4111-B544-BF187DA961CA}"/>
+    <hyperlink ref="E49" r:id="rId51" xr:uid="{7DE18E10-E292-4F66-93C6-F9F900A6FBE1}"/>
+    <hyperlink ref="E50" r:id="rId52" xr:uid="{469E0C85-A97D-4C0E-A1F7-956CA22FCCCB}"/>
+    <hyperlink ref="E51" r:id="rId53" xr:uid="{EE06B41D-7845-490B-99FD-31199829DB2F}"/>
+    <hyperlink ref="E52" r:id="rId54" xr:uid="{7D887B65-BF7F-4D3E-B1FC-0296A94E3797}"/>
+    <hyperlink ref="E53:E57" r:id="rId55" display="https://placehold.co/600x400" xr:uid="{EE25D350-A846-41CB-B126-AD2784D27753}"/>
+    <hyperlink ref="E53" r:id="rId56" xr:uid="{E80C0895-28A4-4980-9DE0-7F49F42E1A4E}"/>
+    <hyperlink ref="E54" r:id="rId57" xr:uid="{878EC35F-9644-4B2B-947A-1E8FB2414B91}"/>
+    <hyperlink ref="E55" r:id="rId58" xr:uid="{8CE7DBCC-ADA5-4314-8DF0-E1621B570FCE}"/>
+    <hyperlink ref="E56" r:id="rId59" xr:uid="{77E1EC7B-37E9-4191-AEAD-6FF3DE513472}"/>
+    <hyperlink ref="E57" r:id="rId60" xr:uid="{8C4ECC5D-4E19-44E5-B08B-E47B53098812}"/>
+    <hyperlink ref="E58" r:id="rId61" xr:uid="{F5BD1B6F-F57D-4096-B3C5-D418A873F778}"/>
+    <hyperlink ref="E59:E62" r:id="rId62" display="images1\facilities\IT\IT_1.webp" xr:uid="{F032E44D-3B3D-4246-8F3A-8C285BF11217}"/>
+    <hyperlink ref="E59" r:id="rId63" xr:uid="{91902898-0448-4215-856A-7BE307EEBACC}"/>
+    <hyperlink ref="E60" r:id="rId64" xr:uid="{E5218CED-E2C4-4D44-950A-30462AFEB678}"/>
+    <hyperlink ref="E61" r:id="rId65" xr:uid="{3F114FFA-23B5-4C72-8564-D4C3CBA186DD}"/>
+    <hyperlink ref="E62" r:id="rId66" xr:uid="{85A98C95-D334-4D7E-B870-F5DA40F70494}"/>
+    <hyperlink ref="E63:E65" r:id="rId67" display="https://placehold.co/600x400" xr:uid="{9AF17048-2561-48B1-89B0-B59B93ECD7AC}"/>
+    <hyperlink ref="E63" r:id="rId68" xr:uid="{0ACDA8AF-D0CF-417C-9AC4-F6877AE5CC91}"/>
+    <hyperlink ref="E64" r:id="rId69" xr:uid="{F764D87F-ACA3-4057-B681-44AACB8946E9}"/>
+    <hyperlink ref="E65" r:id="rId70" xr:uid="{79B97E68-0B65-4E55-848C-99DCA9DFF100}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId69"/>
+  <pageSetup orientation="portrait" r:id="rId71"/>
 </worksheet>
 </file>
</xml_diff>